<commit_message>
Create Data Dictionary from DMN & BPMN models
</commit_message>
<xml_diff>
--- a/dmnClient.Test/TestData/dmnTest1.xlsx
+++ b/dmnClient.Test/TestData/dmnTest1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Arkitektum\DmnClient\dmnClient.Test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8093AE1-AC25-4E9B-8115-CD531D46773C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D82F8D9-724B-4B59-BBEC-44BB1DDCF017}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>DMN Navn:</t>
   </si>
@@ -85,9 +85,6 @@
     <t>out3</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>&lt; 500</t>
   </si>
   <si>
@@ -155,13 +152,25 @@
   </si>
   <si>
     <t>åæø</t>
+  </si>
+  <si>
+    <t>Annotation 02</t>
+  </si>
+  <si>
+    <t>Annotation 04</t>
+  </si>
+  <si>
+    <t>Annotation 05</t>
+  </si>
+  <si>
+    <t>Annotation 06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -582,21 +591,21 @@
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="7" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15.75">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="15.75">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -612,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -638,7 +647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -664,7 +673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -686,108 +695,118 @@
       <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" t="s">
-        <v>44</v>
+      <c r="I11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>